<commit_message>
Modified my schedule and changed the dictionary of old files.
</commit_message>
<xml_diff>
--- a/2019-2020 2nd semester schedule.xlsx
+++ b/2019-2020 2nd semester schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C094AFC-34FE-4B21-AD00-42F425997FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D6D29-312A-4333-A270-0B1FC50D55BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="92">
   <si>
     <t/>
   </si>
@@ -54,9 +54,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>02月17日</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
   </si>
   <si>
     <t>19</t>
-  </si>
-  <si>
-    <t>06月22日</t>
   </si>
   <si>
     <t>上课教室</t>
@@ -473,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -499,16 +493,16 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,13 +511,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -846,7 +846,7 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29:R34"/>
+      <selection activeCell="D8" activeCellId="1" sqref="D5 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -858,60 +858,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
     </row>
     <row r="3" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -924,64 +924,64 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="W3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -992,61 +992,61 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="T4" s="18">
+        <v>44004</v>
+      </c>
+      <c r="U4" s="18">
+        <v>44011</v>
       </c>
       <c r="V4" s="3" t="s">
         <v>0</v>
@@ -1056,64 +1056,64 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>47</v>
+      <c r="A5" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>63</v>
+      <c r="D5" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="9" t="s">
-        <v>71</v>
+      <c r="N5" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="9" t="s">
-        <v>72</v>
+      <c r="R5" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="W5" s="16" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1122,121 +1122,121 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="9"/>
+      <c r="W6" s="12"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="16" t="s">
-        <v>68</v>
+      <c r="F7" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W7" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="W7" s="12"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>67</v>
+      <c r="D8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W8" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="W8" s="12"/>
     </row>
     <row r="9" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1245,31 +1245,31 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-      <c r="W9" s="9"/>
+      <c r="W9" s="12"/>
     </row>
     <row r="10" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1278,64 +1278,64 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="9"/>
+      <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>54</v>
+      <c r="A11" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>63</v>
+      <c r="D11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O11" s="1"/>
@@ -1346,50 +1346,50 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W11" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:23" ht="24" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="N12" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="16" t="s">
-        <v>65</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1397,23 +1397,23 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="W12" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="W12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="16" t="s">
-        <v>61</v>
+      <c r="E13" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="16" t="s">
-        <v>61</v>
+      <c r="G13" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1421,7 +1421,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="9" t="s">
+      <c r="N13" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O13" s="1"/>
@@ -1432,14 +1432,14 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="W13" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="W13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1452,7 +1452,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O14" s="1"/>
@@ -1463,12 +1463,12 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="W14" s="9"/>
+      <c r="W14" s="12"/>
     </row>
     <row r="15" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1477,15 +1477,15 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>63</v>
+      <c r="J15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O15" s="1"/>
@@ -1496,14 +1496,14 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W15" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="W15" s="12"/>
     </row>
     <row r="16" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1513,12 +1513,12 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="16" t="s">
-        <v>62</v>
+      <c r="K16" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="9" t="s">
+      <c r="N16" s="12" t="s">
         <v>0</v>
       </c>
       <c r="O16" s="1"/>
@@ -1529,16 +1529,16 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="W16" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="W16" s="12"/>
     </row>
     <row r="17" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>55</v>
+      <c r="A17" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1560,34 +1560,34 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="9"/>
+      <c r="W17" s="12"/>
     </row>
     <row r="18" spans="1:23" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="16" t="s">
-        <v>61</v>
+      <c r="F18" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>63</v>
+      <c r="H18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1599,14 +1599,14 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="W18" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="W18" s="12"/>
     </row>
     <row r="19" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1628,12 +1628,12 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="W19" s="9"/>
+      <c r="W19" s="12"/>
     </row>
     <row r="20" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1647,32 +1647,32 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="16" t="s">
-        <v>65</v>
+      <c r="O20" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="P20" s="1"/>
-      <c r="Q20" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="R20" s="16" t="s">
+      <c r="Q20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="S20" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="T20" s="16" t="s">
-        <v>63</v>
+      <c r="R20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="U20" s="1"/>
       <c r="V20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W20" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="W20" s="12"/>
     </row>
     <row r="21" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1681,11 +1681,11 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21" s="16" t="s">
-        <v>63</v>
+      <c r="J21" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1698,14 +1698,14 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W21" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1715,8 +1715,8 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="16" t="s">
-        <v>62</v>
+      <c r="K22" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1729,35 +1729,35 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="W22" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="W22" s="12"/>
     </row>
     <row r="23" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>56</v>
+      <c r="A23" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>63</v>
+      <c r="D23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1770,27 +1770,27 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="9" t="s">
-        <v>74</v>
+      <c r="U23" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="W23" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="W23" s="12"/>
     </row>
     <row r="24" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="16" t="s">
-        <v>68</v>
+      <c r="E24" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="16" t="s">
-        <v>68</v>
+      <c r="G24" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1805,52 +1805,52 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-      <c r="U24" s="9" t="s">
+      <c r="U24" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="W24" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="W24" s="12"/>
     </row>
     <row r="25" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" s="15" t="s">
-        <v>63</v>
+      <c r="D25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1858,18 +1858,18 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="9" t="s">
+      <c r="U25" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="W25" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="W25" s="12"/>
     </row>
     <row r="26" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1881,32 +1881,32 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="N26" s="16" t="s">
-        <v>63</v>
+      <c r="M26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="16" t="s">
-        <v>69</v>
+      <c r="P26" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="9" t="s">
+      <c r="U26" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W26" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="W26" s="12"/>
     </row>
     <row r="27" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1920,34 +1920,34 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="16" t="s">
-        <v>69</v>
+      <c r="O27" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="P27" s="1"/>
-      <c r="Q27" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="R27" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="S27" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="T27" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="U27" s="9" t="s">
+      <c r="Q27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="U27" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W27" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="W27" s="12"/>
     </row>
     <row r="28" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1967,18 +1967,18 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="9" t="s">
+      <c r="U28" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V28" s="1"/>
-      <c r="W28" s="9"/>
+      <c r="W28" s="12"/>
     </row>
     <row r="29" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>57</v>
+      <c r="A29" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1988,60 +1988,60 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="9" t="s">
-        <v>70</v>
+      <c r="K29" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="L29" s="1"/>
-      <c r="M29" s="9" t="s">
-        <v>71</v>
+      <c r="M29" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-      <c r="U29" s="9" t="s">
+      <c r="U29" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V29" s="1"/>
-      <c r="W29" s="9"/>
+      <c r="W29" s="12"/>
     </row>
     <row r="30" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K30" s="9" t="s">
+      <c r="D30" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L30" s="1"/>
-      <c r="M30" s="9" t="s">
+      <c r="M30" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N30" s="1"/>
@@ -2053,52 +2053,52 @@
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-      <c r="U30" s="9" t="s">
+      <c r="U30" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="W30" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="W30" s="12"/>
     </row>
     <row r="31" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N31" s="15" t="s">
-        <v>64</v>
+      <c r="D31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -2108,18 +2108,18 @@
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-      <c r="U31" s="9" t="s">
+      <c r="U31" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="W31" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="W31" s="12"/>
     </row>
     <row r="32" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2129,11 +2129,11 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="9" t="s">
+      <c r="K32" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L32" s="1"/>
-      <c r="M32" s="9" t="s">
+      <c r="M32" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N32" s="1"/>
@@ -2145,16 +2145,16 @@
       </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="U32" s="9" t="s">
+      <c r="U32" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V32" s="1"/>
-      <c r="W32" s="9"/>
+      <c r="W32" s="12"/>
     </row>
     <row r="33" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2164,11 +2164,11 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="9" t="s">
+      <c r="K33" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L33" s="1"/>
-      <c r="M33" s="9" t="s">
+      <c r="M33" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N33" s="1"/>
@@ -2180,16 +2180,16 @@
       </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="U33" s="9" t="s">
+      <c r="U33" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V33" s="1"/>
-      <c r="W33" s="9"/>
+      <c r="W33" s="12"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2199,11 +2199,11 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="9" t="s">
+      <c r="K34" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L34" s="1"/>
-      <c r="M34" s="9" t="s">
+      <c r="M34" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N34" s="1"/>
@@ -2215,18 +2215,18 @@
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-      <c r="U34" s="9" t="s">
+      <c r="U34" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V34" s="1"/>
-      <c r="W34" s="9"/>
+      <c r="W34" s="12"/>
     </row>
     <row r="35" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
-        <v>58</v>
+      <c r="A35" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2234,15 +2234,15 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="9" t="s">
-        <v>75</v>
+      <c r="I35" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="J35" s="1"/>
-      <c r="K35" s="9" t="s">
+      <c r="K35" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L35" s="1"/>
-      <c r="M35" s="9" t="s">
+      <c r="M35" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N35" s="1"/>
@@ -2252,16 +2252,16 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-      <c r="U35" s="9" t="s">
+      <c r="U35" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V35" s="1"/>
-      <c r="W35" s="9"/>
+      <c r="W35" s="12"/>
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2269,15 +2269,15 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J36" s="1"/>
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L36" s="1"/>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N36" s="1"/>
@@ -2287,16 +2287,16 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-      <c r="U36" s="9" t="s">
+      <c r="U36" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V36" s="1"/>
-      <c r="W36" s="9"/>
+      <c r="W36" s="12"/>
     </row>
     <row r="37" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -2304,19 +2304,19 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J37" s="1"/>
-      <c r="K37" s="9" t="s">
+      <c r="K37" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L37" s="1"/>
-      <c r="M37" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="N37" s="16" t="s">
-        <v>65</v>
+      <c r="M37" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -2324,18 +2324,18 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
-      <c r="U37" s="9" t="s">
+      <c r="U37" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="W37" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="W37" s="12"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2343,15 +2343,15 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J38" s="1"/>
-      <c r="K38" s="9" t="s">
+      <c r="K38" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L38" s="1"/>
-      <c r="M38" s="9" t="s">
+      <c r="M38" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N38" s="1"/>
@@ -2361,16 +2361,16 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
-      <c r="U38" s="9" t="s">
+      <c r="U38" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V38" s="1"/>
-      <c r="W38" s="9"/>
+      <c r="W38" s="12"/>
     </row>
     <row r="39" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2378,15 +2378,15 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J39" s="1"/>
-      <c r="K39" s="9" t="s">
+      <c r="K39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L39" s="1"/>
-      <c r="M39" s="9" t="s">
+      <c r="M39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N39" s="1"/>
@@ -2396,16 +2396,16 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
-      <c r="U39" s="9" t="s">
+      <c r="U39" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V39" s="1"/>
-      <c r="W39" s="9"/>
+      <c r="W39" s="12"/>
     </row>
     <row r="40" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2413,15 +2413,15 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="9" t="s">
+      <c r="I40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J40" s="1"/>
-      <c r="K40" s="9" t="s">
+      <c r="K40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="L40" s="1"/>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N40" s="1"/>
@@ -2431,18 +2431,18 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="9" t="s">
+      <c r="U40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="V40" s="1"/>
-      <c r="W40" s="9"/>
+      <c r="W40" s="12"/>
     </row>
     <row r="41" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>59</v>
+      <c r="A41" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2450,13 +2450,13 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="9" t="s">
+      <c r="M41" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N41" s="1"/>
@@ -2468,14 +2468,14 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="W41" s="9"/>
+        <v>87</v>
+      </c>
+      <c r="W41" s="12"/>
     </row>
     <row r="42" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2483,13 +2483,13 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="9" t="s">
+      <c r="I42" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="9" t="s">
+      <c r="M42" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N42" s="1"/>
@@ -2501,14 +2501,14 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="W42" s="9"/>
+        <v>88</v>
+      </c>
+      <c r="W42" s="12"/>
     </row>
     <row r="43" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2516,13 +2516,13 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="9" t="s">
+      <c r="M43" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N43" s="1"/>
@@ -2534,14 +2534,14 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="W43" s="9"/>
+        <v>89</v>
+      </c>
+      <c r="W43" s="12"/>
     </row>
     <row r="44" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2549,13 +2549,13 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="9" t="s">
+      <c r="I44" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="9" t="s">
+      <c r="M44" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N44" s="1"/>
@@ -2567,14 +2567,14 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="W44" s="9"/>
+        <v>90</v>
+      </c>
+      <c r="W44" s="12"/>
     </row>
     <row r="45" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2582,13 +2582,13 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="9" t="s">
+      <c r="I45" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="9" t="s">
+      <c r="M45" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N45" s="1"/>
@@ -2600,14 +2600,14 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="W45" s="9"/>
+        <v>91</v>
+      </c>
+      <c r="W45" s="12"/>
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="9"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2615,13 +2615,13 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="12" t="s">
         <v>0</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="9" t="s">
+      <c r="M46" s="12" t="s">
         <v>0</v>
       </c>
       <c r="N46" s="1"/>
@@ -2633,42 +2633,37 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
-      <c r="W46" s="9"/>
+      <c r="W46" s="12"/>
     </row>
     <row r="47" spans="1:23" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
-      <c r="W47" s="9"/>
+      <c r="A47" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="12"/>
+      <c r="U47" s="12"/>
+      <c r="V47" s="12"/>
+      <c r="W47" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A16"/>
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A40"/>
@@ -2684,6 +2679,11 @@
     <mergeCell ref="I35:I46"/>
     <mergeCell ref="J5:J10"/>
     <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A16"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>